<commit_message>
corrected format of mapping schemes (Bel, Serb)
</commit_message>
<xml_diff>
--- a/res_mapping_schemes/mapping_Belgium_RES.xlsx
+++ b/res_mapping_schemes/mapping_Belgium_RES.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C9FBEF-179E-5E4F-80C3-EFC68A2B6B11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E83888-A355-9448-8DB4-A0716496A31E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_urban" sheetId="1" r:id="rId1"/>
@@ -23,38 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
-    <t>Multi-family
-before 1945</t>
-  </si>
-  <si>
-    <t>Multi-family
-1946-1970 (early post-war)</t>
-  </si>
-  <si>
-    <t>Multi-family
-1971-2005</t>
-  </si>
-  <si>
-    <t>Multi-family
-after 2006</t>
-  </si>
-  <si>
-    <t>Single-family
-before 1945</t>
-  </si>
-  <si>
-    <t>Single-family
-1946-1970 (early post-war)</t>
-  </si>
-  <si>
-    <t>Single-family
-1971-2005</t>
-  </si>
-  <si>
-    <t>Single-family
-after 2006</t>
-  </si>
-  <si>
     <t>70% CR/LFINF+CDN/HBET:3-5
 30% CR/LWAL+CDN/HBET:3-5</t>
   </si>
@@ -104,14 +72,45 @@
   <si>
     <t>Dwelling type and year of construction</t>
   </si>
+  <si>
+    <t>Multi-family before 1945</t>
+  </si>
+  <si>
+    <t>Multi-family 1946-1970 (early post-war)</t>
+  </si>
+  <si>
+    <t>Multi-family 1971-2005</t>
+  </si>
+  <si>
+    <t>Multi-family after 2006</t>
+  </si>
+  <si>
+    <t>Single-family before 1945</t>
+  </si>
+  <si>
+    <t>Single-family 1946-1970 (early post-war)</t>
+  </si>
+  <si>
+    <t>Single-family 1971-2005</t>
+  </si>
+  <si>
+    <t>Single-family after 2006</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -172,17 +171,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -482,58 +484,58 @@
   <sheetData>
     <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -545,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -561,58 +563,58 @@
   <sheetData>
     <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mapping scheme for Belgium (reduce % W) following local expert feedback
</commit_message>
<xml_diff>
--- a/res_mapping_schemes/mapping_Belgium_RES.xlsx
+++ b/res_mapping_schemes/mapping_Belgium_RES.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10914"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E83888-A355-9448-8DB4-A0716496A31E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC92D66A-AA06-2B40-815E-5F2D340B9067}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_urban" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>70% CR/LFINF+CDN/HBET:3-5
 30% CR/LWAL+CDN/HBET:3-5</t>
@@ -52,12 +52,6 @@
 25% CR+PC/LWAL+CDN/HBET:3-5</t>
   </si>
   <si>
-    <t>40% MUR/LWAL+CDN/H:1
-40% MUR/LWAL+CDN/H:2
-10% W/LWAL+CDN/H:1
-10% W/LWAL+CDN/H:2</t>
-  </si>
-  <si>
     <t>45% MUR/LWAL+CDN/H:1
 45% MUR/LWAL+CDN/H:2
 5% W/LWAL+CDN/H:1
@@ -95,15 +89,32 @@
   </si>
   <si>
     <t>Single-family after 2006</t>
+  </si>
+  <si>
+    <t>50% MUR/LWAL+CDN/H:1
+50% MUR/LWAL+CDN/H:2</t>
+  </si>
+  <si>
+    <t>49% MUR/LWAL+CDN/H:1
+49% MUR/LWAL+CDN/H:2
+1% W/LWAL+CDN/H:1
+1% W/LWAL+CDN/H:2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -171,19 +182,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -468,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -484,31 +498,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -517,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -525,16 +539,16 @@
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -547,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -563,31 +577,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -604,16 +618,16 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>